<commit_message>
django server connect && labeled data preprocess
</commit_message>
<xml_diff>
--- a/xlsx/stats0709.xlsx
+++ b/xlsx/stats0709.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2352,25 +2352,17 @@
           <t>2024-07-09</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>901923</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>15819</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>4273</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>1190000</t>
-        </is>
+      <c r="D26" t="n">
+        <v>901923</v>
+      </c>
+      <c r="E26" t="n">
+        <v>15819</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4273</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1190000</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -2406,6 +2398,1907 @@
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/VWmWScovllY/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>oakQvwCbvr8</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2285883</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2183</v>
+      </c>
+      <c r="F27" t="n">
+        <v>16793</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1600000</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>UCom6YhUY62jM52nIMjf5_dw</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>오킹TV</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>안녕하세요 크리에이터 오킹입니다! 근거없는 낭설/악플, 싸움조장, 해당 영상과 관련없는 댓글 삭제합니다. 각종 공지는 네이버 카페로 오셔서 확인바랍니다.</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Society</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>24년 5월 24일 라이브</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>오킹, 오킹TV, 트위치, 스트리머, 유튜버, 유튜브, 썰스트리머, 일상</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/oakQvwCbvr8/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>-HZeqsIgGHo</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1414201</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3226</v>
+      </c>
+      <c r="F28" t="n">
+        <v>14904</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1600000</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>UCom6YhUY62jM52nIMjf5_dw</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>오킹TV</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>안녕하세요 크리에이터 오킹입니다! 근거없는 낭설/악플, 싸움조장, 해당 영상과 관련없는 댓글 삭제합니다. 각종 공지는 네이버 카페로 오셔서 확인바랍니다.</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Society</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>오킹입니다.</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/-HZeqsIgGHo/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>nAy-7zuCVQs</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2024-02-19</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4439142</v>
+      </c>
+      <c r="E29" t="n">
+        <v>16286</v>
+      </c>
+      <c r="F29" t="n">
+        <v>42408</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1600000</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>UCom6YhUY62jM52nIMjf5_dw</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>오킹TV</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>안녕하세요 크리에이터 오킹입니다! 근거없는 낭설/악플, 싸움조장, 해당 영상과 관련없는 댓글 삭제합니다. 각종 공지는 네이버 카페로 오셔서 확인바랍니다.</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Society</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>위너즈 고소와 못했던 이야기</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>안녕하세요 오킹입니다. 구독자여러분께 현 상황에 대해 평소처럼 조리있게 설명드리고 싶었으나 그러지 못한 점 양해부탁드립니다. 
+영상 전문은 양이 많아 커뮤니티에 올려놓겠습니다.</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>오킹, 오킹TV, 트위치, 스트리머, 유튜버, 유튜브, 썰스트리머, 일상</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/nAy-7zuCVQs/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>QojVuirFx58</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2024-02-08</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4903575</v>
+      </c>
+      <c r="E30" t="n">
+        <v>16227</v>
+      </c>
+      <c r="F30" t="n">
+        <v>37508</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1600000</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>UCom6YhUY62jM52nIMjf5_dw</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>오킹TV</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>안녕하세요 크리에이터 오킹입니다! 근거없는 낭설/악플, 싸움조장, 해당 영상과 관련없는 댓글 삭제합니다. 각종 공지는 네이버 카페로 오셔서 확인바랍니다.</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>안녕하세요 오킹입니다.</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>오킹, 오킹TV, 트위치, 스트리머, 유튜버, 유튜브, 썰스트리머, 일상</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/QojVuirFx58/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ibI5OOZXSj8</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2024-02-05</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1009563</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3966</v>
+      </c>
+      <c r="F31" t="n">
+        <v>7332</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1600000</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>UCom6YhUY62jM52nIMjf5_dw</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>오킹TV</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>안녕하세요 크리에이터 오킹입니다! 근거없는 낭설/악플, 싸움조장, 해당 영상과 관련없는 댓글 삭제합니다. 각종 공지는 네이버 카페로 오셔서 확인바랍니다.</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>남자들끼리의 흔한 대화법</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>◆ 오킹 팬카페! 네이버 카페   : https://oking.kr/fancafe
+◆ 쏠란트 홈페이지 바로가기 : https://ssolant.com
+◆ 오킹에게 후원하기              : https://oking.kr/donate
+◆ 오킹의 생방송 다시보기     : https://oking.kr/youtube2
+◆ 영상 업로드는 매일 18시! 많은 관심 부탁 드릴게요!
+◆ 구독과 좋아요 부탁드립니다.
+근거없는 낭설 / 악플, 싸움조장 댓글 삭제 합니다.
+BY.진교 
+영상 및 광고 문의
+이메일 : okingcompany93@gmail.com
+#오킹 #찐친 #주간핫클립</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>오킹, 오킹TV, 트위치, 스트리머, 유튜버, 유튜브, 썰스트리머, 일상</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/ibI5OOZXSj8/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>g5KDoSqT24Q</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2024-07-06</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>85345</v>
+      </c>
+      <c r="E32" t="n">
+        <v>718</v>
+      </c>
+      <c r="F32" t="n">
+        <v>289</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1270000</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>UC8a6z7i9qypp9PqJ_0HhBrw</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>깡스타일리스트</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">관리하는 남자 스타일리스트 '깡' 입니다. 
+패션과 헤어 관리에 미쳐 있으며, 
+남자에 관한 모든것을 리뷰하고 진심으로 영상을 만듭니다. 
+#패션
+#그루밍
+#헤어
+#브이로그 
+</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Fashion, https://en.wikipedia.org/wiki/Lifestyle_(sociology)</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>여학생 대부분이 공감하는 여름신발 1위</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>#여름코디 #신발  #남자패션 
+─────────더보기란────────────
+(해당 영상은 협찬 및 ppl과 관련이 없음을 알려드립니다)
+0:00 인트로
+0:13 오프닝
+0:47 게스트소개
+2:26 버켄스탁 &amp; 츄바스코
+5:38 헌터 &amp; 아디다스
+7:47 필로모티 &amp; 로스트가든
+10:32 나이키 &amp; 크록스
+13:04 살로몬 &amp; 나이키
+15:23 다음 영상 예고
+비지니스 메일 : ad@kkst.kr
+kkst cs 메일 : cs@kkst.kr
+네이버 카페  https://cafe.naver.com/kkangstylist
+인스타그램  https://instagram.com/kkang.stylist
+솔로탈출 출연신청: https://forms.gle/LREiiqrcBaRdQb1D6</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>깡스타일리스트, 남자패션유튜버, 남자코디, 남자패션, 스트릿패션, 미니멀패션, 남친룩, 캐주얼패션, 남자캐주얼, 남자미니멀룩, 남자데이트룩, 남자바지, 니트, 남자니트, 남자코트, 코트추천, 싱글코트, 더블코트, 발마칸코트, 캐주얼룩, 미니멀룩, 여자들이좋아하는, 나이대별, 유행, 오버핏, 2024, 트렌드, 패션, 미니멀, 나이키, 아디다스, 코트, 남자옷, 안경, 뿔테, 청바지, 이너, 나시, 셔츠, 긴팔티, 롱슬리브, 아우터, 봄, 가디건, 기본템, 필수템, 패션레벨, 우선순위, 여름, 반팔, 반바지, 후드티, 바람막이, 다이어트, 양말, 반팔티, 버뮤다팬츠, 무신사, 후드집업, 모자, 스투시, 백팩, 가방, 남자반팔, 맨투맨, 카고팬츠, 린넨셔츠, 데님셔츠, 반팔셔츠, 반팔니트, 슬리퍼, 신발, 운동화, 초여름, 스트릿, 캐주얼, 가성비, 옷장, 카라티, 피그먼트, 선블리치, 추천, 오버핏반팔, 남자여름패션, 반팔추천, 코디, 깡, 깡스, 스타일리스트깡, 여자들이 싫어하는, 최악, 극혐, 여름패션, 인터뷰, 꿀팁, 바지, 반스, 아식스, 쿠어, 남자브랜드, 데일리룩, 코디모음, 룩북, ootd, 뉴발란스, 크록스, 버뮤다, 칼하트, 와이드팬츠, 슬랙스, 콜라보</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/g5KDoSqT24Q/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>mnn1_yu0aDQ</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2024-07-04</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>51274</v>
+      </c>
+      <c r="E33" t="n">
+        <v>553</v>
+      </c>
+      <c r="F33" t="n">
+        <v>163</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1270000</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>UC8a6z7i9qypp9PqJ_0HhBrw</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>깡스타일리스트</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">관리하는 남자 스타일리스트 '깡' 입니다. 
+패션과 헤어 관리에 미쳐 있으며, 
+남자에 관한 모든것을 리뷰하고 진심으로 영상을 만듭니다. 
+#패션
+#그루밍
+#헤어
+#브이로그 
+</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Fashion, https://en.wikipedia.org/wiki/Lifestyle_(sociology)</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>사장님이 미쳤다…제 소장품 3000벌 풉니다.</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>#플리마켓 #시즌오프 #블랙프라이데이 
+─────────더보기란────────────
+(해당 영상은 협찬 및 ppl과 관련이 없음을 알려드립니다)
+비지니스 메일 : ad@kkst.kr
+kkst cs 메일 : cs@kkst.kr
+네이버 카페  https://cafe.naver.com/kkangstylist
+인스타그램  https://instagram.com/kkang.stylist
+스타일 변신 프로젝트 지원: https://forms.gle/iQkDJrjyFv3tfw7b7​</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>깡스타일리스트, 남자패션유튜버, 남자코디, 남자패션, 스트릿패션, 미니멀패션, 남친룩, 캐주얼패션, 남자캐주얼, 남자미니멀룩, 남자데이트룩, 남자바지, 캐주얼룩, 미니멀룩, 여자들이좋아하는, 나이대별, 유행, 2024, 트렌드, 패션, 미니멀, 나이키, 아디다스, 코트, 남자옷, 안경, 뿔테, 청바지, 이너, 나시, 셔츠, 긴팔티, 롱슬리브, 아우터, 봄, 가디건, 기본템, 필수템, 패션레벨, 우선순위, 여름, 반팔, 반바지, 후드티, 바람막이, 다이어트, 양말, 반팔티, 버뮤다팬츠, 무신사, 후드집업, 모자, 스투시, 백팩, 가방, 남자반팔, 맨투맨, 카고팬츠, 린넨셔츠, 데님셔츠, 반팔셔츠, 반팔니트, 슬리퍼, 신발, 운동화, 초여름, 스트릿, 캐주얼, 가성비, 옷장, 제모, 선크림, 관리, 남자관리, 동기부여, 자기계발, 남자신발, 트레통, 장화, 레인부츠, 장마신발, 로스트가든, 시즌오프, 할인, 악세사리, 니트, 겨울옷, 무진장, 블랙프라이데이, 지갑, 빅세일, zara, 유니클로, hm, 감사제</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/mnn1_yu0aDQ/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>pp_C0MGj9ZM</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2024-07-03</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>72225</v>
+      </c>
+      <c r="E34" t="n">
+        <v>947</v>
+      </c>
+      <c r="F34" t="n">
+        <v>120</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1270000</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>UC8a6z7i9qypp9PqJ_0HhBrw</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>깡스타일리스트</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">관리하는 남자 스타일리스트 '깡' 입니다. 
+패션과 헤어 관리에 미쳐 있으며, 
+남자에 관한 모든것을 리뷰하고 진심으로 영상을 만듭니다. 
+#패션
+#그루밍
+#헤어
+#브이로그 
+</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Fashion, https://en.wikipedia.org/wiki/Lifestyle_(sociology)</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>유니클로 세일할때 사야하는 필수템 10가지</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>#블랙프라이데이 #시즌오프 #유니클로 
+─────────더보기란────────────
+(해당 영상은 협찬 및 ppl과 관련이 없음을 알려드립니다)
+00:00 오프닝
+01:08 유니클로 쇼핑
+16:01 H&amp;M 쇼핑
+23:19 엔딩
+비지니스 메일 : ad@kkst.kr
+kkst cs 메일 : cs@kkst.kr
+네이버 카페  https://cafe.naver.com/kkangstylist
+인스타그램  https://instagram.com/kkang.stylist
+스타일 변신 프로젝트 지원: https://forms.gle/iQkDJrjyFv3tfw7b7​</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>깡스타일리스트, 남자패션유튜버, 남자코디, 남자패션, 스트릿패션, 미니멀패션, 남친룩, 캐주얼패션, 남자캐주얼, 남자미니멀룩, 남자데이트룩, 남자바지, 캐주얼룩, 미니멀룩, 여자들이좋아하는, 나이대별, 유행, 2024, 트렌드, 패션, 미니멀, 나이키, 아디다스, 코트, 남자옷, 안경, 뿔테, 청바지, 이너, 나시, 셔츠, 긴팔티, 롱슬리브, 아우터, 봄, 가디건, 기본템, 필수템, 패션레벨, 우선순위, 여름, 반팔, 반바지, 후드티, 바람막이, 다이어트, 양말, 반팔티, 버뮤다팬츠, 무신사, 후드집업, 모자, 스투시, 백팩, 가방, 남자반팔, 맨투맨, 카고팬츠, 린넨셔츠, 데님셔츠, 반팔셔츠, 반팔니트, 슬리퍼, 신발, 운동화, 초여름, 스트릿, 캐주얼, 가성비, 옷장, 제모, 선크림, 관리, 남자관리, 동기부여, 자기계발, 남자신발, 트레통, 장화, 레인부츠, 장마신발, 로스트가든, 시즌오프, 할인, 악세사리, 니트, 겨울옷, 무진장, 블랙프라이데이, 지갑, 빅세일, zara, 유니클로, hm, 감사제</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/pp_C0MGj9ZM/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>_Otk-iMD_X0</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2024-07-02</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>59163</v>
+      </c>
+      <c r="E35" t="n">
+        <v>647</v>
+      </c>
+      <c r="F35" t="n">
+        <v>62</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1270000</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>UC8a6z7i9qypp9PqJ_0HhBrw</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>깡스타일리스트</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">관리하는 남자 스타일리스트 '깡' 입니다. 
+패션과 헤어 관리에 미쳐 있으며, 
+남자에 관한 모든것을 리뷰하고 진심으로 영상을 만듭니다. 
+#패션
+#그루밍
+#헤어
+#브이로그 
+</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Fashion, https://en.wikipedia.org/wiki/Lifestyle_(sociology)</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>7월, 미친 날씨 옷잘알의 여름 코디 꿀팁</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>#여름코디 #흰티 #반팔
+─────────더보기란────────────
+(해당 영상은 협찬 및 ppl과 관련이 없음을 알려드립니다)
+00:00 오프닝
+00:16 흰 티 활용법
+06:19 셔츠 활용법
+10:05 연예인코디 / 봉태규
+10:43 연예인코디 / 김원중
+11:36 연예인코디 / 준호
+12:02 연예인코디 / 류준열
+12:25 엔딩
+비지니스 메일 : ad@kkst.kr
+kkst cs 메일 : cs@kkst.kr
+네이버 카페  https://cafe.naver.com/kkangstylist
+인스타그램  https://instagram.com/kkang.stylist
+스타일 변신 프로젝트 지원: https://forms.gle/iQkDJrjyFv3tfw7b7​</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>깡스타일리스트, 남자패션유튜버, 남자코디, 남자패션, 스트릿패션, 미니멀패션, 남친룩, 캐주얼패션, 남자캐주얼, 남자미니멀룩, 남자데이트룩, 남자바지, 니트, 남자니트, 남자코트, 코트추천, 싱글코트, 더블코트, 발마칸코트, 캐주얼룩, 미니멀룩, 여자들이좋아하는, 나이대별, 유행, 오버핏, 2024, 트렌드, 패션, 미니멀, 나이키, 아디다스, 코트, 남자옷, 안경, 뿔테, 청바지, 이너, 나시, 셔츠, 긴팔티, 롱슬리브, 아우터, 봄, 가디건, 기본템, 필수템, 패션레벨, 우선순위, 여름, 반팔, 반바지, 후드티, 바람막이, 다이어트, 양말, 반팔티, 버뮤다팬츠, 무신사, 후드집업, 모자, 스투시, 백팩, 가방, 남자반팔, 맨투맨, 카고팬츠, 린넨셔츠, 데님셔츠, 반팔셔츠, 반팔니트, 슬리퍼, 신발, 운동화, 초여름, 스트릿, 캐주얼, 가성비, 옷장</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/_Otk-iMD_X0/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>_HZ63R-8z4E</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>57530</v>
+      </c>
+      <c r="E36" t="n">
+        <v>650</v>
+      </c>
+      <c r="F36" t="n">
+        <v>278</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1270000</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>UC8a6z7i9qypp9PqJ_0HhBrw</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>깡스타일리스트</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">관리하는 남자 스타일리스트 '깡' 입니다. 
+패션과 헤어 관리에 미쳐 있으며, 
+남자에 관한 모든것을 리뷰하고 진심으로 영상을 만듭니다. 
+#패션
+#그루밍
+#헤어
+#브이로그 
+</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Fashion, https://en.wikipedia.org/wiki/Lifestyle_(sociology)</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>고민할 필요 없습니다.. 3만원으로 실버 악세사리 3종 뽑았다 [콜라보왕] Ep.16</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>#악세사리 #반지 #목걸이
+─────────더보기란────────────
+ 여러분들 의견을 바탕으로 실버소재를 사용했고 목걸이,팔찌,반지 만들었습니다. 잘선택된 악세사리는 평범한 옷도 세련되게 만들어주고 외모도 살려줍니다. 매일 차는 악세사리인 만큼 정성스럽고 자신있게 만들었습니다.
+- 콜라보 제품  바로가기 https://vo.la/ZbQsS
+00:00 오프닝
+00:48 제작과정
+01:28 가격미팅
+08:05 리뷰시작
+09:30 스퀘어 체인 실버 브레이슬릿
+10:01 트위스트 실버 브레이슬릿
+11:12 케이블 체인 실버 네크리스
+11:41 커브 스퀘어 펜던트 실버 네크리스
+12:59 그레디언트 실버 링
+13:49 트위스트 실버 링
+14:18 엔딩
+비지니스 메일 : ad@kkst.kr
+kkst cs 메일 : cs@kkst.kr
+네이버 카페  https://cafe.naver.com/kkangstylist
+인스타그램  https://instagram.com/kkang.stylist
+솔로탈출 출연신청: https://forms.gle/LREiiqrcBaRdQb1D6</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>깡스타일리스트, 남자패션유튜버, 남자코디, 남자패션, 스트릿패션, 미니멀패션, 남친룩, 캐주얼패션, 남자캐주얼, 남자미니멀룩, 남자데이트룩, 남자바지, 캐주얼룩, 미니멀룩, 여자들이좋아하는, 나이대별, 유행, 오버핏, 2024, 트렌드, 패션, 미니멀, 나이키, 아디다스, 올드머니, 남자옷, 안경, 뿔테, 청바지, 봄코디, 인터뷰, 코디, 추천, 꿀팁, 폴로, 무신사, 셔츠, 바지, 반팔, 카고팬츠, 반스, 아식스, 남자브랜드, 긴팔티, 데일리룩, 코디모음, 룩북, 여름, 반팔티, 카라티, 반팔니트, 남자룩북, ootd, 반바지, 셋업, 추리닝, 조거팬츠, 에어리즘, 쿨탠다드, 유니클로, 무신사스탠다드, 쿨에어, 탑텐, spa, 흰티, 무지티, 기능성, 가성비, 티셔츠, 기본템, 기본티, 기본흰티셔츠, 꿀템, 무지반팔, 메르고, KKST, 반팔셔츠, 여름셔츠, 여름바지, 나일론팬츠, 블랙프라이데이, 시즌오프, 반지, 팔찌, 목걸이, 실버, 주얼리, 남자주얼리</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/_HZ63R-8z4E/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>yLlKOd3I8CA</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2024-07-08</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>133145</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1733</v>
+      </c>
+      <c r="F37" t="n">
+        <v>526</v>
+      </c>
+      <c r="G37" t="n">
+        <v>513000</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>UCVJT18d9wSCnDUdnJ9ycO7Q</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>동수칸TV</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">로스트 아크,롤, 풋볼매니저 등 종합게임 방송 한동숙의 칸튜브
+치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+비지니스 문의:  charon@gysent.com
+</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Association_football, https://en.wikipedia.org/wiki/Sport</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>갑자기 한국 축구 국대 감독에 홍명보???</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>#축협 #축구 #국가대표 
+▶치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+▶인스타그램 https://www.instagram.com/woooookhan
+▶롱수칸 https://www.youtube.com/@longsukhan
+▶네이버 카페 https://cafe.naver.com/khantata
+ * 좋아요 버튼과 구독 버튼을 눌러주셔서 
+    감사합니다! 열심히 하겠습니다!
+ * 댓글로 허위사실 및 심한 욕설시 
+    무통보 삭제될 수 있음을 알려드립니다.</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>게임, 한동숙, 칸튜브, 동수칸, ㄷㅅㅋ</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/yLlKOd3I8CA/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BYWO-z-4tfo</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2024-07-08</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>144835</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1323</v>
+      </c>
+      <c r="F38" t="n">
+        <v>170</v>
+      </c>
+      <c r="G38" t="n">
+        <v>513000</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>UCVJT18d9wSCnDUdnJ9ycO7Q</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>동수칸TV</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">로스트 아크,롤, 풋볼매니저 등 종합게임 방송 한동숙의 칸튜브
+치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+비지니스 문의:  charon@gysent.com
+</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Action-adventure_game, https://en.wikipedia.org/wiki/Action_game, https://en.wikipedia.org/wiki/Role-playing_video_game, https://en.wikipedia.org/wiki/Video_game_culture</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>진격의 드라이버 괴물쥐</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>#현현공공 #체인드투게더 #ChainedTogether #칸튜브 
+▶치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+▶인스타그램 https://www.instagram.com/woooookhan
+▶롱수칸 https://www.youtube.com/@longsukhan
+▶네이버 카페 https://cafe.naver.com/khantata
+ * 좋아요 버튼과 구독 버튼을 눌러주셔서 
+    감사합니다! 열심히 하겠습니다!
+ * 댓글로 허위사실 및 심한 욕설시 
+    무통보 삭제될 수 있음을 알려드립니다.</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>게임, 한동숙, 칸튜브, 동수칸, ㄷㅅㅋ</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/BYWO-z-4tfo/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>uNq7RMRwIHs</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2024-07-07</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>201626</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1988</v>
+      </c>
+      <c r="F39" t="n">
+        <v>177</v>
+      </c>
+      <c r="G39" t="n">
+        <v>513000</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>UCVJT18d9wSCnDUdnJ9ycO7Q</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>동수칸TV</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">로스트 아크,롤, 풋볼매니저 등 종합게임 방송 한동숙의 칸튜브
+치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+비지니스 문의:  charon@gysent.com
+</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Action-adventure_game, https://en.wikipedia.org/wiki/Action_game, https://en.wikipedia.org/wiki/Casual_game, https://en.wikipedia.org/wiki/Role-playing_video_game, https://en.wikipedia.org/wiki/Video_game_culture</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>얘네는 왜 하루 종일 떨어짐?</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>#현현공공 #체인드투게더 #ChainedTogether #칸튜브 
+▶치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+▶인스타그램 https://www.instagram.com/woooookhan
+▶롱수칸 https://www.youtube.com/@longsukhan
+▶네이버 카페 https://cafe.naver.com/khantata
+ * 좋아요 버튼과 구독 버튼을 눌러주셔서 
+    감사합니다! 열심히 하겠습니다!
+ * 댓글로 허위사실 및 심한 욕설시 
+    무통보 삭제될 수 있음을 알려드립니다.
+-
+[출처] 코코넛콘 블로그, 환영해요 로아콘! 
+(https://blog.daum.net/coconut-emoji/107)</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>게임, 한동숙, 칸튜브, 동수칸, ㄷㅅㅋ</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/uNq7RMRwIHs/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ZLXz98YW_U0</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2024-07-05</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>336335</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2672</v>
+      </c>
+      <c r="F40" t="n">
+        <v>167</v>
+      </c>
+      <c r="G40" t="n">
+        <v>513000</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>UCVJT18d9wSCnDUdnJ9ycO7Q</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>동수칸TV</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">로스트 아크,롤, 풋볼매니저 등 종합게임 방송 한동숙의 칸튜브
+치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+비지니스 문의:  charon@gysent.com
+</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Action-adventure_game, https://en.wikipedia.org/wiki/Action_game, https://en.wikipedia.org/wiki/Role-playing_video_game, https://en.wikipedia.org/wiki/Video_game_culture</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>로아 시즌3 트레일러 동수칸 반응</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>#로스트아크 #로아 #시즌3 #칸튜브 
+▶치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+▶인스타그램 https://www.instagram.com/woooookhan
+▶롱수칸 https://www.youtube.com/@longsukhan
+▶네이버 카페 https://cafe.naver.com/khantata
+ * 좋아요 버튼과 구독 버튼을 눌러주셔서 
+    감사합니다! 열심히 하겠습니다!
+ * 댓글로 허위사실 및 심한 욕설시 
+    무통보 삭제될 수 있음을 알려드립니다.</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>게임, 한동숙, 칸튜브, 동수칸, ㄷㅅㅋ</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/ZLXz98YW_U0/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>qkXc1M3d7g4</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2024-07-05</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>185332</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1660</v>
+      </c>
+      <c r="F41" t="n">
+        <v>125</v>
+      </c>
+      <c r="G41" t="n">
+        <v>513000</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>UCVJT18d9wSCnDUdnJ9ycO7Q</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>동수칸TV</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">로스트 아크,롤, 풋볼매니저 등 종합게임 방송 한동숙의 칸튜브
+치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+비지니스 문의:  charon@gysent.com
+</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Action_game, https://en.wikipedia.org/wiki/Casual_game, https://en.wikipedia.org/wiki/Role-playing_video_game, https://en.wikipedia.org/wiki/Video_game_culture</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>한결같은 우리 삼식이</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>#프로젝트윈터 #마피아게임 #산악회 #칸튜브 
+▶치지직 생방송  https://chzzk.naver.com/75cbf189b3bb8f9f687d2aca0d0a382b
+▶인스타그램 https://www.instagram.com/woooookhan
+▶롱수칸 https://www.youtube.com/@longsukhan
+▶네이버 카페 https://cafe.naver.com/khantata
+ * 좋아요 버튼과 구독 버튼을 눌러주셔서 
+    감사합니다! 열심히 하겠습니다!
+ * 댓글로 허위사실 및 심한 욕설시 
+    무통보 삭제될 수 있음을 알려드립니다.
+-
+Music provided by 브금대통령
+Track : 인생 뭐 있냐 - https://youtu.be/EJR1MutUW9o
+Track : Green n Red - https://youtu.be/j8YNfm_lBAQ
+Track : 비틀비틀 - https://youtu.be/kkTYGStJ968
+Track : Mr. Scrooge - https://youtu.be/KHR2IcENsqc
+-
+[출처] 코코넛콘 블로그, 환영해요 로아콘! 
+(https://blog.daum.net/coconut-emoji/107)</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>게임, 한동숙, 칸튜브, 동수칸, ㄷㅅㅋ</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/qkXc1M3d7g4/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>-rHqqCxjhM4</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2024-07-08</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>30216</v>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>54</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1520000</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>UCg86gCCgZGWkoHk8c015cQQ</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>때잉</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>나만 알고 싶은데 다들 알았으면 좋겠다
+📧 sttaeing@gmail.com</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Music, https://en.wikipedia.org/wiki/Pop_music</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>03년생이 말아주는 03년도 감성ִ𖤐💖 : The Kid LAROI - GIRLS [가사/해석/lyrics]</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>With SONY MUSIC KOREA
+#03  #라로이 #스테이걔 
+상당한 인소 감성의 가사입니다 
+스파이더맨을 바라보는 아이언맨의 기분이 이런 걸까
+현지에서는 비버 데뷔초 느낌 난다는 의견이 대부분이네ㅇㅕ
+🎬Spring Breakers
+이 채널은 영상의 조회수로 수익을 창출하지 않습니다.
+THIS CHANNEL DOESN'T GENERATE REVENUE.
+このチャンネルは収益を生み出しません。
+CONTACT
+📧 sttaeing@gmail.com
+📧Instagram : https://www.instagram.com/sttayingg?igsh=NHZ4NzF6cG9lZDF2&amp;utm_source=qr</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>때잉, 팝송, 노래, 플레이리스트, playlist, pop, 가사해석, 가사, 영화, movie, netflix, 넷플릭스</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/-rHqqCxjhM4/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>FGjrtBFgTXY</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2024-06-29</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>104211</v>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>98</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1520000</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>UCg86gCCgZGWkoHk8c015cQQ</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>때잉</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>나만 알고 싶은데 다들 알았으면 좋겠다
+📧 sttaeing@gmail.com</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Music, https://en.wikipedia.org/wiki/Music_of_Asia, https://en.wikipedia.org/wiki/Pop_music</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>🔥수상할 정도로 좋은 노래만 뽑음 : H1-KEY(하이키) - 뜨거워지자 [가사/Eng/Kor]</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>#하이키
+건사피장의 하이키입니다 저는 항상... 노래가 좋아야 뜬다에 한 표 거는 사람입니다
+🎬 소년시절의 너 (2019)
+지원을 받아 제작된 영상입니다.:) 
+영상의 조회수로 수익을 창출하지 않습니다. (This channel doesn't generate revenue)
+인스타그램 https://www.instagram.com/sttayingg?igsh=NHZ4NzF6cG9lZDF2&amp;utm_source=qr</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>때잉, 팝송, 노래, 플레이리스트, playlist, pop, 가사해석, 가사, 영화, movie, netflix, 넷플릭스</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/FGjrtBFgTXY/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>TOSrdHy5KRc</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2024-06-24</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>252516</v>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="n">
+        <v>243</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1520000</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>UCg86gCCgZGWkoHk8c015cQQ</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>때잉</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>나만 알고 싶은데 다들 알았으면 좋겠다
+📧 sttaeing@gmail.com</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Independent_music, https://en.wikipedia.org/wiki/Music, https://en.wikipedia.org/wiki/Pop_music, https://en.wikipedia.org/wiki/Rock_music</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>도입부터 매운맛 때려박고 시작🚨: Måneskin - I WANNA BE YOUR SLAVE (가사/해석/lyrics)</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>#모네스킨
+노예가 되... 주인님이 되.... 
+🎬기묘한 이야기 S03  
+with Sony Music Korea   
+영상의 조회수로 수익을 창출하지 않습니다. (This channel doesn't generate revenue)
+인스타그램 https://www.instagram.com/sttayingg?igsh=NHZ4NzF6cG9lZDF2&amp;utm_source=qr</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>때잉, 팝송, 노래, 플레이리스트, playlist, pop, 가사해석, 가사, 영화, movie, netflix, 넷플릭스</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/TOSrdHy5KRc/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>wdUu3XQK8cE</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>57025</v>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="n">
+        <v>101</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1520000</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>UCg86gCCgZGWkoHk8c015cQQ</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>때잉</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>나만 알고 싶은데 다들 알았으면 좋겠다
+📧 sttaeing@gmail.com</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Electronic_music, https://en.wikipedia.org/wiki/Music, https://en.wikipedia.org/wiki/Pop_music, https://en.wikipedia.org/wiki/Soul_music</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>🥃𝐃𝐏𝐑 𝐈𝐀𝐍이 직접 고른, 잭다니엘스 향 진하게 나는 𝐩𝐥𝐚𝐲𝐥𝐢𝐬𝐭🎵</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>잭 다니엘스 x 때잉
+DPR IAN에게 영감이 되어준 음악들을 잭 다니엘스 한잔과 함께 즐겨보세요.
+𝐔𝐧𝐩𝐥𝐮𝐠 𝐰𝐢𝐭𝐡 𝐌𝐮𝐬𝐢𝐜. 𝐉𝐚𝐜𝐤 𝐃𝐚𝐧𝐢𝐞𝐥'𝐬. 
+🥃 모델을 어떻게 이렇게 찰떡으로 골랐나요
+잭다니엘로 개명하셔도 되겠음
++ 저는 사실 양주파인데요 최근에 잭다니엘스 애플도 마셔봤는데 괜찮았음
+#잭다니엘스 #dprian 
+영상의 조회수로 수익을 창출하지 않습니다. (This channel doesn't generate revenue)
+인스타그램 https://www.instagram.com/sttayingg?igsh=NHZ4NzF6cG9lZDF2&amp;utm_source=qr</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>때잉, 팝송, 노래, 플레이리스트, playlist, pop, 가사해석, 가사, 영화, movie, netflix, 넷플릭스, 때껄룩, Takealook, 치명플리, 위스키</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/wdUu3XQK8cE/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>LamRCcz4zqg</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2024-06-16</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>152163</v>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="n">
+        <v>134</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1520000</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>UCg86gCCgZGWkoHk8c015cQQ</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>때잉</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>나만 알고 싶은데 다들 알았으면 좋겠다
+📧 sttaeing@gmail.com</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Music, https://en.wikipedia.org/wiki/Pop_music</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>한국 노랜 줄 또 나만 몰랐지.. 🫢 : eldon - Fraud [가사/해석/lyrics]</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>#엘던 
+사실 나는 알고 있었다
+🎬 : Time Freak
+지원을 받아 제작된 영상입니다. :)
+영상의 조회수로 수익을 창출하지 않습니다. (This channel doesn't generate revenue)
+인스타그램 https://www.instagram.com/sttayingg?igsh=NHZ4NzF6cG9lZDF2&amp;utm_source=qr</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>때잉, 팝송, 노래, 플레이리스트, playlist, pop, 가사해석, 가사, 영화, movie, netflix, 넷플릭스</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/LamRCcz4zqg/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ahcPfSLbT-M</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2024-07-08</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>679082</v>
+      </c>
+      <c r="E47" t="n">
+        <v>12164</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2579</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1190000</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>UClE2hKVqycauBKmXwawizEg</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>뻑가 PPKKa</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>제가 하고싶은 말과 생각입니다</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>한숨</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>유튜브후원 https://www.youtube.com/channel/UClE2hKVqycauBKmXwawizEg/join
+이메일 ppkka.hello@gmail.com
+후원하기 https://toon.at/donate/ppkka</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/ahcPfSLbT-M/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>8l4GZ4datyM</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2024-07-07</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>512518</v>
+      </c>
+      <c r="E48" t="n">
+        <v>10285</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1942</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1190000</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>UClE2hKVqycauBKmXwawizEg</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>뻑가 PPKKa</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>제가 하고싶은 말과 생각입니다</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Society</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>목적 달성했다는 이유</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>유튜브후원 https://www.youtube.com/channel/UClE2hKVqycauBKmXwawizEg/join
+이메일 ppkka.hello@gmail.com
+후원하기 https://toon.at/donate/ppkka</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/8l4GZ4datyM/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>7I790Er-zkc</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2024-07-06</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1073236</v>
+      </c>
+      <c r="E49" t="n">
+        <v>14399</v>
+      </c>
+      <c r="F49" t="n">
+        <v>4693</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1190000</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>UClE2hKVqycauBKmXwawizEg</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>뻑가 PPKKa</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>제가 하고싶은 말과 생각입니다</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Society</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>엮이면 x되는 여자들(2부)</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>유튜브후원 https://www.youtube.com/channel/UClE2hKVqycauBKmXwawizEg/join
+이메일 ppkka.hello@gmail.com
+후원하기 https://toon.at/donate/ppkka</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/7I790Er-zkc/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>8SJs1Cg7hpU</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2024-07-06</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>633911</v>
+      </c>
+      <c r="E50" t="n">
+        <v>9205</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2293</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1190000</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>UClE2hKVqycauBKmXwawizEg</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>뻑가 PPKKa</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>제가 하고싶은 말과 생각입니다</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>좀 별로네(1부)</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>유튜브후원 https://www.youtube.com/channel/UClE2hKVqycauBKmXwawizEg/join
+이메일 ppkka.hello@gmail.com
+후원하기 https://toon.at/donate/ppkka</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>https://i.ytimg.com/vi/8SJs1Cg7hpU/default.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>VWmWScovllY</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2024-07-04</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>902067</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>15821</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>4275</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>1190000</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>UClE2hKVqycauBKmXwawizEg</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>뻑가 PPKKa</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>제가 하고싶은 말과 생각입니다</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Society</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>120만 유튜버 인지능력</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>유튜브후원 https://www.youtube.com/channel/UClE2hKVqycauBKmXwawizEg/join
+이메일 ppkka.hello@gmail.com
+후원하기 https://toon.at/donate/ppkka</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr">
         <is>
           <t>https://i.ytimg.com/vi/VWmWScovllY/default.jpg</t>
         </is>

</xml_diff>